<commit_message>
A shit ton of work that should have been done on seperate commits, but oh well
</commit_message>
<xml_diff>
--- a/assets/minecraft/models/item/log.xlsx
+++ b/assets/minecraft/models/item/log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devon\AppData\Roaming\.minecraft\resourcepacks\Delve Resources\assets\delve\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devon\AppData\Roaming\.minecraft\resourcepacks\Delve Resources\assets\minecraft\models\item\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594EAF83-2473-46A9-AC0E-EB6DF03C7078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469B3EF0-2476-45D1-B357-831CCA2D81B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="28770" windowHeight="15570" xr2:uid="{BF6163C6-360E-4628-B4D7-86628954E740}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF6163C6-360E-4628-B4D7-86628954E740}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>01</t>
   </si>
@@ -235,6 +235,12 @@
   </si>
   <si>
     <t>stone_door_small_1</t>
+  </si>
+  <si>
+    <t>potion</t>
+  </si>
+  <si>
+    <t>pendulum</t>
   </si>
 </sst>
 </file>
@@ -263,7 +269,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,6 +299,12 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -307,7 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -325,6 +337,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -652,7 +667,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,8 +725,8 @@
       <c r="G2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>61</v>
+      <c r="H2" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>69</v>
@@ -736,8 +751,8 @@
       <c r="G3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>62</v>
+      <c r="H3" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -747,6 +762,9 @@
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C4" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="E4" s="6" t="s">
         <v>64</v>
       </c>
@@ -756,11 +774,14 @@
       <c r="G4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>66</v>
+      <c r="H4" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>70</v>
+      </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added spike plate model
</commit_message>
<xml_diff>
--- a/assets/minecraft/models/item/log.xlsx
+++ b/assets/minecraft/models/item/log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devon\AppData\Roaming\.minecraft\resourcepacks\Delve Resources\assets\minecraft\models\item\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469B3EF0-2476-45D1-B357-831CCA2D81B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F092E5A-2A71-4DD8-9030-60E2418C4FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF6163C6-360E-4628-B4D7-86628954E740}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>01</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>pendulum</t>
+  </si>
+  <si>
+    <t>spike plate extend</t>
+  </si>
+  <si>
+    <t>spike plate retract</t>
   </si>
 </sst>
 </file>
@@ -667,7 +673,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,6 +791,9 @@
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C5" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="G5" s="3" t="s">
         <v>58</v>
       </c>
@@ -792,6 +801,9 @@
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Added Golden Goblet treasure type
</commit_message>
<xml_diff>
--- a/assets/minecraft/models/item/log.xlsx
+++ b/assets/minecraft/models/item/log.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devon\AppData\Roaming\.minecraft\resourcepacks\Delve Resources\assets\minecraft\models\item\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F092E5A-2A71-4DD8-9030-60E2418C4FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF25041-25AE-41AA-AF9E-13DCACFDAD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF6163C6-360E-4628-B4D7-86628954E740}"/>
+    <workbookView xWindow="30" yWindow="345" windowWidth="28770" windowHeight="15255" xr2:uid="{BF6163C6-360E-4628-B4D7-86628954E740}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>01</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>spike plate retract</t>
+  </si>
+  <si>
+    <t>golden_goblet</t>
+  </si>
+  <si>
+    <t>silver goblet?</t>
   </si>
 </sst>
 </file>
@@ -673,7 +679,7 @@
   <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,10 +819,16 @@
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G7" s="3" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added moving platforms and abyss_tiles
</commit_message>
<xml_diff>
--- a/assets/minecraft/models/item/log.xlsx
+++ b/assets/minecraft/models/item/log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devon\AppData\Roaming\.minecraft\resourcepacks\Delve Resources\assets\minecraft\models\item\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F092E5A-2A71-4DD8-9030-60E2418C4FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAE9B40-0641-4344-ACD1-E7AD46C35FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BF6163C6-360E-4628-B4D7-86628954E740}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>01</t>
   </si>
@@ -247,6 +247,18 @@
   </si>
   <si>
     <t>spike plate retract</t>
+  </si>
+  <si>
+    <t>00 (utility)</t>
+  </si>
+  <si>
+    <t>stained_glass</t>
+  </si>
+  <si>
+    <t>abyss_tile</t>
+  </si>
+  <si>
+    <t>rusty_platform_double</t>
   </si>
 </sst>
 </file>
@@ -275,7 +287,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,6 +323,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -325,7 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -348,6 +366,9 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -357,6 +378,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF66CC"/>
       <color rgb="FFD7A78D"/>
       <color rgb="FFFF6600"/>
       <color rgb="FFFF7C80"/>
@@ -670,191 +692,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7645412C-85F6-40D2-A071-82B61EFD1780}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="22" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" style="1"/>
-    <col min="2" max="2" width="18.85546875" style="2"/>
-    <col min="3" max="16384" width="18.85546875" style="1"/>
+    <col min="1" max="1" width="22" style="1"/>
+    <col min="2" max="2" width="8" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22" style="2"/>
+    <col min="4" max="16384" width="22" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" s="2">
         <v>255</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>75</v>
+      </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D7" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>